<commit_message>
Adapt R preprocessing to changes in py import and ampliseq output
Melting/unpivoting (wide) asv-table to (long) occurrence tbl in py/pandas is too slow for larger datasets. Until I rewrite the import script, I use data.table melt in R do do this before py import.
</commit_message>
<xml_diff>
--- a/scripts/processing/input/reannotation.xlsx
+++ b/scripts/processing/input/reannotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/scripts/processing/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385026A8-F775-CE41-854A-4891FC04BE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE857C93-CD97-CF4E-B901-23EB8CB3EC6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16820" yWindow="7760" windowWidth="31480" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16220" yWindow="17320" windowWidth="34380" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="annotation" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="63">
   <si>
     <t>asv_sequence</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Assigned kingdom OR barrnap-positive</t>
   </si>
   <si>
-    <t>TTCACGATGGTGATCCCTGTTTATATGGCGCTTTACATGAACAAATTTCCCGTTTAGCTGATGCTGGCATTGAAGTTGAAGTTATACCTGGTATTAGTGCCTATCAAGCAACAGCAGCAGCGCTTGGGGCTGAATTAACAATTCCTGGGCTCGTGCAAACAATTGTTCTAAGCCGCGCCAGCGGGCGCACCGGCACACCAGCTCGCGAATCTTTAGCGCACATAGCAGCTCTTGGTGCTTCTCTCTGCCTTTATCTAAGCGCCCGCCATGTGGAAGAGGTTGAAGCGATATTGCTGCAACATTAC</t>
-  </si>
-  <si>
     <t>TCGAGAATTTTTCACAATGGGGGAAACCCTGATGGAGCGACGCCGCGTGGAGGATGAAGGTTTTCGGATTGTAAACTCCTGTCATTAGAGAACAAGGCACATGGTTTAACTGGCCGTGTGTTGATAGTATCTGAAGAGGAAGGGACGGCTAACTCTGTGCCAGCAGCCGCGGTAATACAGAGGTCTCAAGCGTTGTTCGGATTCATTGGGCGTAAAGGGTGCGTAGGTGGCGAGGTAAGTCGGATGTGAAATCTCCAAGCTCAACTTGGAAACTGCATTCGATACTGCTTTGCTAGAGGATTGTAGAGGGCATTGGAATTCACGGTGTAGCAGTGAAATGCGTAGATATCGTGAGGAAGACCAGTGGCGAAGGCGAATGCCTGGGCAATTCCTGACACTGAGGCACGAAGGCCAGGGGAGCAAACG</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>Chthoniobacterales</t>
   </si>
   <si>
-    <t>UBA6821</t>
-  </si>
-  <si>
     <t>TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTTTTACAAGTCTGTCGTTAAAACGTGGAGCTCAACTCCATTTCGGCGATGGAAACTGTAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCTAGGGGAGCGAAAG</t>
   </si>
   <si>
@@ -206,6 +200,15 @@
   </si>
   <si>
     <t>Planktophila</t>
+  </si>
+  <si>
+    <t>Terrimicrobiaceae</t>
+  </si>
+  <si>
+    <t>Terrimicrobium</t>
+  </si>
+  <si>
+    <t>Unassigned</t>
   </si>
 </sst>
 </file>
@@ -1055,13 +1058,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="54" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1129,35 +1135,35 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>39</v>
+      <c r="A2" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="2">
-        <v>44609</v>
+        <v>45103</v>
       </c>
       <c r="N2" t="s">
         <v>19</v>
@@ -1182,35 +1188,35 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>44</v>
+      <c r="A3" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L3" t="s">
         <v>6</v>
       </c>
       <c r="M3" s="2">
-        <v>44609</v>
+        <v>45103</v>
       </c>
       <c r="N3" t="s">
         <v>19</v>
@@ -1235,29 +1241,20 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>50</v>
+      <c r="A4" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M4" s="2">
-        <v>44609</v>
+        <v>45103</v>
       </c>
       <c r="N4" t="s">
         <v>19</v>
@@ -1275,15 +1272,15 @@
         <v>36</v>
       </c>
       <c r="T4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>51</v>
+      <c r="A5" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -1292,25 +1289,25 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
         <v>52</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>53</v>
       </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
       <c r="K5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L5" t="s">
         <v>6</v>
       </c>
       <c r="M5" s="2">
-        <v>44609</v>
+        <v>45103</v>
       </c>
       <c r="N5" t="s">
         <v>19</v>
@@ -1335,35 +1332,35 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>56</v>
+      <c r="A6" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>46</v>
       </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>48</v>
-      </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L6" t="s">
         <v>6</v>
       </c>
       <c r="M6" s="2">
-        <v>44609</v>
+        <v>45103</v>
       </c>
       <c r="N6" t="s">
         <v>19</v>
@@ -1388,8 +1385,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>58</v>
+      <c r="A7" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -1398,25 +1395,25 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>53</v>
       </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" t="s">
-        <v>55</v>
-      </c>
       <c r="K7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L7" t="s">
         <v>6</v>
       </c>
       <c r="M7" s="2">
-        <v>44609</v>
+        <v>45103</v>
       </c>
       <c r="N7" t="s">
         <v>19</v>
@@ -1441,7 +1438,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" t="s">
@@ -1472,7 +1469,7 @@
         <v>30</v>
       </c>
       <c r="M8" s="2">
-        <v>44609</v>
+        <v>45103</v>
       </c>
       <c r="N8" t="s">
         <v>19</v>
@@ -1497,7 +1494,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B9" t="s">
@@ -1525,7 +1522,7 @@
         <v>6</v>
       </c>
       <c r="M9" s="2">
-        <v>44609</v>
+        <v>45103</v>
       </c>
       <c r="N9" t="s">
         <v>19</v>
@@ -1550,32 +1547,32 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>59</v>
+      <c r="A10" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L10" t="s">
         <v>5</v>
       </c>
       <c r="M10" s="2">
-        <v>44609</v>
+        <v>45103</v>
       </c>
       <c r="N10" t="s">
         <v>19</v>
@@ -1600,8 +1597,8 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>60</v>
+      <c r="A11" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -1610,25 +1607,25 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
         <v>52</v>
       </c>
-      <c r="E11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" t="s">
-        <v>54</v>
-      </c>
       <c r="G11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L11" t="s">
         <v>6</v>
       </c>
       <c r="M11" s="2">
-        <v>44609</v>
+        <v>45103</v>
       </c>
       <c r="N11" t="s">
         <v>19</v>
@@ -1640,53 +1637,15 @@
         <v>21</v>
       </c>
       <c r="Q11">
-        <v>0.99</v>
+        <v>0.4</v>
       </c>
       <c r="S11" t="s">
         <v>36</v>
       </c>
       <c r="T11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="2">
-        <v>44609</v>
-      </c>
-      <c r="N12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12" t="s">
-        <v>20</v>
-      </c>
-      <c r="P12" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q12">
-        <v>0.99</v>
-      </c>
-      <c r="S12" t="s">
-        <v>36</v>
-      </c>
-      <c r="T12" t="b">
-        <v>1</v>
-      </c>
-      <c r="U12" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>